<commit_message>
T360-593: Simulate concurrent WhatsApp notification requests
Updated the test to simulate 3 parallel requests per test case and validate that only one is successful while others are rejected, reflecting concurrency handling. Enhanced result export with additional fields, updated the Excel interface, changed the test data sheet, and fixed the output filename for invalid notification tests.
</commit_message>
<xml_diff>
--- a/src/testData/archivosExcel/TestCasesNotificacionesParalelo.xlsx
+++ b/src/testData/archivosExcel/TestCasesNotificacionesParalelo.xlsx
@@ -7,6 +7,8 @@
     <sheet state="visible" name="Test2" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Test3" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Test4" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Test5" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Test6" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="4">
   <si>
     <t>CELULAR</t>
   </si>
@@ -32,7 +34,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -49,6 +51,10 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -64,7 +70,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -76,6 +82,15 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -98,6 +113,14 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -7379,4 +7402,398 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.64301298E8</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.64301298E8</v>
+      </c>
+      <c r="C3" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="D3" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.64301298E8</v>
+      </c>
+      <c r="C4" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="D4" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.64301298E8</v>
+      </c>
+      <c r="C5" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="D5" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.64301298E8</v>
+      </c>
+      <c r="C6" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="D6" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.64301298E8</v>
+      </c>
+      <c r="C7" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="D7" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.64301312E8</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.64301312E8</v>
+      </c>
+      <c r="C9" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="D9" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.64301312E8</v>
+      </c>
+      <c r="C10" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="D10" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.64301312E8</v>
+      </c>
+      <c r="C11" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="D11" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.64301312E8</v>
+      </c>
+      <c r="C12" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="D12" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.64301312E8</v>
+      </c>
+      <c r="C13" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="D13" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.64301313E8</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D2" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.64301313E8</v>
+      </c>
+      <c r="C3" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="D3" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.64301313E8</v>
+      </c>
+      <c r="C4" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="D4" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.64301313E8</v>
+      </c>
+      <c r="C5" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="D5" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.64301313E8</v>
+      </c>
+      <c r="C6" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="D6" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.64301313E8</v>
+      </c>
+      <c r="C7" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="D7" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.64301314E8</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.64301314E8</v>
+      </c>
+      <c r="C9" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="D9" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.64301314E8</v>
+      </c>
+      <c r="C10" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="D10" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.64301314E8</v>
+      </c>
+      <c r="C11" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="D11" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.64301314E8</v>
+      </c>
+      <c r="C12" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="D12" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4">
+        <v>9.26208479E8</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.64301314E8</v>
+      </c>
+      <c r="C13" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="D13" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>